<commit_message>
test and burndown chart
</commit_message>
<xml_diff>
--- a/scrum/burndown_template.xlsx
+++ b/scrum/burndown_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kayle\cs3250\project-3-student-management-blueteam\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD0DC71-EE72-4D99-8987-95C59E90D38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E92FB83-2B6C-413A-BC20-C25F6C6DDDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="792" windowWidth="12672" windowHeight="11172" xr2:uid="{7A4C5A10-B1D5-9946-8D6C-7E3C0798020F}"/>
+    <workbookView xWindow="708" yWindow="1068" windowWidth="16524" windowHeight="11172" xr2:uid="{7A4C5A10-B1D5-9946-8D6C-7E3C0798020F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,6 +377,12 @@
                 <c:pt idx="0">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -432,7 +438,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -472,10 +478,10 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1590,7 +1596,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1636,8 +1642,12 @@
       <c r="C3" s="4">
         <v>6</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="4">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -1654,7 +1664,7 @@
       </c>
       <c r="E4" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1671,11 +1681,11 @@
       </c>
       <c r="D5" s="4">
         <f t="shared" ref="D5:E5" si="1">C5-D3</f>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>